<commit_message>
refactor: update template Warm Up
</commit_message>
<xml_diff>
--- a/docs/warmUp/template_PlanCalentamiento-WarmUp.xlsx
+++ b/docs/warmUp/template_PlanCalentamiento-WarmUp.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcosLambirTorres\Dev\SFMC\docs\warmUp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C1A5E42-A87A-415C-BB6A-E2D3E9DF3835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{127E71A9-F945-4BFA-8FA9-7AA62FF69046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="WU ENDESA" sheetId="1" r:id="rId1"/>
+    <sheet name="WU TEMPLATE" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="44">
   <si>
     <t>Plan de calentamiento IP - ENDESA</t>
   </si>
@@ -41,9 +41,6 @@
     <t>CREATIVIDAD</t>
   </si>
   <si>
-    <t>CONTACTABLES</t>
-  </si>
-  <si>
     <t>Dia 1</t>
   </si>
   <si>
@@ -86,9 +83,6 @@
     <t>Creatividad 4</t>
   </si>
   <si>
-    <t>BASE DE DATOS (DE_WU_2024)</t>
-  </si>
-  <si>
     <t xml:space="preserve">	&lt;cantidad&gt;</t>
   </si>
   <si>
@@ -128,19 +122,49 @@
     <t>&lt;Positiva, Negativa&gt;</t>
   </si>
   <si>
-    <t>&lt;el día de la creatividad&gt;</t>
-  </si>
-  <si>
     <t>TOTAL ENVIOS:</t>
   </si>
   <si>
-    <t>*Se incrementan los Envíos diarios según la tabla oficial de Salesforce</t>
-  </si>
-  <si>
     <t>Envio diario</t>
   </si>
   <si>
     <t>Envioo diario</t>
+  </si>
+  <si>
+    <t>*Se incrementan los Envíos diarios en base a la tabla oficial de Salesforce. El fin es llegar a realizar un envío total de toda la DE (tabla) dentro de las 5 semanas del Warm Up.</t>
+  </si>
+  <si>
+    <t>&lt;- Objetivo de Envío</t>
+  </si>
+  <si>
+    <t>&lt;Día de la Creatividad&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Total DE&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Envío según Salesforce&gt;</t>
+  </si>
+  <si>
+    <t>*La respuesta será positiva o negativa dependiendo de la buena recepción de los Subscribers.</t>
+  </si>
+  <si>
+    <t>Día 2</t>
+  </si>
+  <si>
+    <t>Día 3</t>
+  </si>
+  <si>
+    <t>&lt;Creatividad&gt;</t>
+  </si>
+  <si>
+    <t>CONTACTABLES:</t>
+  </si>
+  <si>
+    <t>TABLA (DE_WU_2024):</t>
+  </si>
+  <si>
+    <t>*Cuando se terminan los Split de la DE para realizar envíos a todos los Subscribers, se vuelve a empezar para llegar al envío objetivo (el de toda la DE).</t>
   </si>
 </sst>
 </file>
@@ -150,7 +174,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,8 +253,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="24">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -363,14 +395,8 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -448,11 +474,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -550,12 +585,6 @@
     <xf numFmtId="0" fontId="4" fillId="22" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="23" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -570,6 +599,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -788,34 +832,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="35.54296875" customWidth="1"/>
-    <col min="2" max="2" width="19.6328125" customWidth="1"/>
-    <col min="3" max="3" width="19.7265625" customWidth="1"/>
-    <col min="4" max="4" width="19.6328125" customWidth="1"/>
-    <col min="5" max="6" width="19.7265625" customWidth="1"/>
-    <col min="7" max="8" width="13.6328125" customWidth="1"/>
-    <col min="9" max="9" width="19.7265625" customWidth="1"/>
-    <col min="10" max="12" width="10.7265625" customWidth="1"/>
+    <col min="2" max="6" width="21.6328125" customWidth="1"/>
+    <col min="7" max="8" width="11.1796875" customWidth="1"/>
+    <col min="9" max="10" width="21.6328125" customWidth="1"/>
+    <col min="11" max="12" width="10.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -831,16 +873,16 @@
     <row r="4" spans="1:10" ht="14.5" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="14.5" x14ac:dyDescent="0.35"/>
@@ -869,16 +911,22 @@
       <c r="H9" s="12">
         <v>45603</v>
       </c>
-      <c r="I9" s="40"/>
-      <c r="J9" s="41"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="39"/>
     </row>
     <row r="10" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
+      <c r="B10" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>12</v>
+      </c>
       <c r="E10" s="30"/>
       <c r="F10" s="32"/>
       <c r="G10" s="14"/>
@@ -886,38 +934,42 @@
     </row>
     <row r="11" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" s="13">
-        <v>11</v>
+        <v>30</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>36</v>
       </c>
       <c r="C11" s="13">
-        <v>21</v>
+        <v>500</v>
       </c>
       <c r="D11" s="13">
-        <v>31</v>
+        <v>500</v>
       </c>
       <c r="E11" s="13"/>
       <c r="F11" s="15"/>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
-      <c r="I11" s="37">
+      <c r="I11" s="35">
         <f>SUM(B11:F11)</f>
-        <v>63</v>
-      </c>
-      <c r="J11" s="38"/>
+        <v>1000</v>
+      </c>
+      <c r="J11" s="36"/>
     </row>
     <row r="12" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A12" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
+        <v>18</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
       <c r="G12" s="16"/>
       <c r="H12" s="16"/>
     </row>
@@ -959,7 +1011,7 @@
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="10" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B15" s="13"/>
       <c r="C15" s="15"/>
@@ -968,15 +1020,15 @@
       <c r="F15" s="13"/>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
-      <c r="I15" s="37">
+      <c r="I15" s="35">
         <f>SUM(B15:F15)</f>
         <v>0</v>
       </c>
-      <c r="J15" s="38"/>
+      <c r="J15" s="36"/>
     </row>
     <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -1024,7 +1076,7 @@
     </row>
     <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B19" s="13"/>
       <c r="C19" s="15"/>
@@ -1033,21 +1085,21 @@
       <c r="F19" s="13"/>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
-      <c r="I19" s="37">
+      <c r="I19" s="35">
         <f>SUM(B19:F19)</f>
         <v>0</v>
       </c>
-      <c r="J19" s="38"/>
+      <c r="J19" s="36"/>
     </row>
     <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
+        <v>18</v>
+      </c>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
       <c r="G20" s="16"/>
       <c r="H20" s="16"/>
     </row>
@@ -1089,7 +1141,7 @@
     </row>
     <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B23" s="13"/>
       <c r="C23" s="15"/>
@@ -1098,21 +1150,21 @@
       <c r="F23" s="13"/>
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
-      <c r="I23" s="37">
+      <c r="I23" s="35">
         <f>SUM(B23:F23)</f>
         <v>0</v>
       </c>
-      <c r="J23" s="38"/>
+      <c r="J23" s="36"/>
     </row>
     <row r="24" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
+        <v>18</v>
+      </c>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
       <c r="G24" s="16"/>
       <c r="H24" s="16"/>
     </row>
@@ -1147,157 +1199,175 @@
       <c r="B26" s="29"/>
       <c r="C26" s="30"/>
       <c r="D26" s="29"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="29"/>
+      <c r="E26" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="43" t="s">
+        <v>33</v>
+      </c>
       <c r="G26" s="14"/>
       <c r="H26" s="14"/>
     </row>
     <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B27" s="13"/>
       <c r="C27" s="15"/>
       <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
+      <c r="E27" s="15" t="s">
+        <v>35</v>
+      </c>
       <c r="F27" s="15"/>
       <c r="G27" s="14"/>
       <c r="H27" s="14"/>
-      <c r="I27" s="37">
+      <c r="I27" s="35">
         <f>SUM(B27:F27)</f>
         <v>0</v>
       </c>
-      <c r="J27" s="38"/>
+      <c r="J27" s="36"/>
     </row>
     <row r="28" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
+        <v>18</v>
+      </c>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24">
+        <v>16</v>
+      </c>
+      <c r="F28" s="24"/>
       <c r="G28" s="16"/>
       <c r="H28" s="16"/>
     </row>
     <row r="29" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="B29" s="36"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="36"/>
-      <c r="I29" s="36"/>
-      <c r="J29" s="36"/>
+      <c r="A29" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
     </row>
     <row r="30" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" s="41"/>
+      <c r="C30" s="41"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="41"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="42"/>
       <c r="I30" s="20" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="J30" s="19">
         <f>SUM(I11:I27)</f>
-        <v>63</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="32" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="18"/>
       <c r="B32" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C32" s="21" t="s">
+      <c r="D32" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="D32" s="21" t="s">
+      <c r="E32" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E32" s="21" t="s">
+      <c r="F32" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="F32" s="21" t="s">
-        <v>7</v>
-      </c>
       <c r="L32" s="2"/>
     </row>
-    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B33" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C33" s="22" t="s">
+      <c r="F33" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D33" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="E33" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="F33" s="23" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B34" s="24" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C34" s="24"/>
       <c r="D34" s="24"/>
       <c r="E34" s="24"/>
       <c r="F34" s="24"/>
     </row>
-    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="6"/>
       <c r="B36" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="C36" s="21" t="s">
+      <c r="D36" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D36" s="21" t="s">
+      <c r="E36" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="E36" s="21" t="s">
+      <c r="F36" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="F36" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B37" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C37" s="25" t="s">
+      <c r="E37" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="D37" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="E37" s="26" t="s">
-        <v>16</v>
-      </c>
       <c r="F37" s="26" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B38" s="24"/>
       <c r="C38" s="24"/>
@@ -1305,48 +1375,48 @@
       <c r="E38" s="24"/>
       <c r="F38" s="24"/>
     </row>
-    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="6"/>
       <c r="B40" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C40" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D40" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C40" s="21" t="s">
+      <c r="E40" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="D40" s="21" t="s">
+      <c r="F40" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="E40" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="F40" s="21" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="41" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B41" s="27" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C41" s="27" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D41" s="26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E41" s="27" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F41" s="27" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B42" s="24"/>
       <c r="C42" s="24"/>
@@ -1354,38 +1424,38 @@
       <c r="E42" s="24"/>
       <c r="F42" s="24"/>
     </row>
-    <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="44" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="6"/>
       <c r="B44" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C44" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D44" s="21" t="s">
         <v>27</v>
-      </c>
-      <c r="C44" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="D44" s="21" t="s">
-        <v>29</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
     </row>
-    <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B45" s="27" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C45" s="27" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D45" s="28"/>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
     </row>
-    <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B46" s="24"/>
       <c r="C46" s="24"/>
@@ -1393,11 +1463,21 @@
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
     </row>
-    <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-    </row>
-    <row r="48" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="47" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="44" t="s">
+        <v>37</v>
+      </c>
+      <c r="B47" s="44"/>
+      <c r="C47" s="44"/>
+      <c r="D47" s="44"/>
+      <c r="E47" s="44"/>
+      <c r="F47" s="44"/>
+      <c r="G47" s="44"/>
+      <c r="H47" s="44"/>
+      <c r="I47" s="44"/>
+      <c r="J47" s="44"/>
+    </row>
+    <row r="48" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="49" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="50" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="51" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2351,18 +2431,20 @@
     <row r="999" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="1000" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
+    <mergeCell ref="A47:J47"/>
     <mergeCell ref="A29:J29"/>
     <mergeCell ref="I23:J23"/>
     <mergeCell ref="I27:J27"/>
-    <mergeCell ref="A1:I1"/>
     <mergeCell ref="I9:J9"/>
     <mergeCell ref="I11:J11"/>
     <mergeCell ref="I15:J15"/>
     <mergeCell ref="I19:J19"/>
+    <mergeCell ref="A30:H30"/>
+    <mergeCell ref="A1:J1"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>